<commit_message>
modified to print class-specific accuracies
</commit_message>
<xml_diff>
--- a/Alex Code/Results/03042019/ExpLog.xlsx
+++ b/Alex Code/Results/03042019/ExpLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexw\Documents\GitHub\ARMS\Alex Code\Results\03042019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0674D1B-097F-4723-9A20-89103D5820FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B82AD5F-BF1C-4666-B0C3-E48D6AB66C2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1656" yWindow="924" windowWidth="17280" windowHeight="8964" xr2:uid="{EC48ED26-35B8-4B02-97AB-6316AB7EB481}"/>
+    <workbookView xWindow="936" yWindow="3996" windowWidth="17280" windowHeight="8964" xr2:uid="{EC48ED26-35B8-4B02-97AB-6316AB7EB481}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7A5AC9-A5C0-473C-AC68-9AA3E698FC96}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,6 +504,32 @@
         <v>0.94120000000000004</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="F4">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.85189999999999999</v>
+      </c>
+      <c r="H4">
+        <v>0.91180000000000005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>